<commit_message>
Added consensus fasta file
</commit_message>
<xml_diff>
--- a/output/assembly/assembly_stats.xlsx
+++ b/output/assembly/assembly_stats.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/Documents/Grad_School/Research/Assembly/PhaeobacterS4Sm-genome-assembly/output/assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60542460-E346-E043-A3FC-71520A4A6B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6B46D1-2074-704A-B660-39C9AEE70F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{93048B7B-EE35-484E-8BF6-AE56F7762AE6}"/>
+    <workbookView xWindow="480" yWindow="1560" windowWidth="27640" windowHeight="16440" xr2:uid="{93048B7B-EE35-484E-8BF6-AE56F7762AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>A:</t>
   </si>
@@ -202,19 +204,157 @@
   </si>
   <si>
     <t>Raven</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs P_tig00000001</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs Q_contig_1</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs R_Utg8118</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs S_tig00000001</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs T_contig_1</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs U_Utg7924</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs V_tig00000001</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs W_contig_1</t>
+  </si>
+  <si>
+    <t>O_Utg7906 vs X_Utg8092</t>
+  </si>
+  <si>
+    <t>Comparison</t>
+  </si>
+  <si>
+    <t>Overall-identity</t>
+  </si>
+  <si>
+    <t>Worst-1kbp-identity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    99.975% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     99.975% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    99.974% </t>
+  </si>
+  <si>
+    <t>Total length (&gt;= 50000 bp)</t>
+  </si>
+  <si>
+    <t>Largest contig</t>
+  </si>
+  <si>
+    <t>Total length</t>
+  </si>
+  <si>
+    <t>Estimated reference length</t>
+  </si>
+  <si>
+    <t>GC (%)</t>
+  </si>
+  <si>
+    <t>N50</t>
+  </si>
+  <si>
+    <t>NG50</t>
+  </si>
+  <si>
+    <t>N90</t>
+  </si>
+  <si>
+    <t>NG90</t>
+  </si>
+  <si>
+    <t>auN</t>
+  </si>
+  <si>
+    <t>auNG</t>
+  </si>
+  <si>
+    <t>L50</t>
+  </si>
+  <si>
+    <t>LG50</t>
+  </si>
+  <si>
+    <t>L90</t>
+  </si>
+  <si>
+    <t>LG90</t>
+  </si>
+  <si>
+    <t>Assembly                       </t>
+  </si>
+  <si>
+    <t>consensus</t>
+  </si>
+  <si>
+    <t>4179+2part</t>
+  </si>
+  <si>
+    <t>3773+2part</t>
+  </si>
+  <si>
+    <t>511+1part</t>
+  </si>
+  <si>
+    <t>49+0part</t>
+  </si>
+  <si>
+    <t>contigs (&gt;= 50000 bp)</t>
+  </si>
+  <si>
+    <t>contigs</t>
+  </si>
+  <si>
+    <t>N's per 100 kbp</t>
+  </si>
+  <si>
+    <t>predicted genes (unique)</t>
+  </si>
+  <si>
+    <t>predicted genes (&gt;= 0 bp)</t>
+  </si>
+  <si>
+    <t>predicted genes (&gt;= 300 bp)</t>
+  </si>
+  <si>
+    <t>predicted genes (&gt;= 1500 bp)</t>
+  </si>
+  <si>
+    <t>predicted genes (&gt;= 3000 bp)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,7 +365,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -233,13 +373,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +726,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -997,4 +1166,345 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A72EC2-EC45-D84F-AA99-BAF78D525AB8}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.99975000000000003</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.99975000000000003</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.99975000000000003</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0F4FC1-1D7E-3149-90D8-C0CB01A95A5B}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4385166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3951184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4385166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4400000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="7">
+        <v>59.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="7">
+        <v>3951184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3951184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="7">
+        <v>3951184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="7">
+        <v>291202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="7">
+        <v>3581816.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="7">
+        <v>3569741.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="7">
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>